<commit_message>
añadido el diagrama de bd
</commit_message>
<xml_diff>
--- a/documentacion/Backlog.xlsx
+++ b/documentacion/Backlog.xlsx
@@ -489,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -528,182 +528,190 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="105">
-      <c r="A5" s="4">
+    <row r="5" spans="1:6">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="105">
+      <c r="A6" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45">
-      <c r="A6" s="4">
+    <row r="7" spans="1:6" ht="45">
+      <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B7" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60">
-      <c r="A7" s="4">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4">
-        <v>3</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="60">
       <c r="A8" s="4">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="60">
+      <c r="A9" s="4">
         <v>2</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B9" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" ht="30">
-      <c r="A9" s="4">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="30">
+      <c r="A10" s="4">
         <v>5</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B10" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="105">
-      <c r="A10" s="4">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="105">
+      <c r="A11" s="4">
         <v>6</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B11" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="30">
-      <c r="A11" s="4">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="30">
+      <c r="A12" s="4">
         <v>7</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B12" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="B14" t="s">
+    <row r="15" spans="1:6">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
         <v>2</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B20" s="1">
         <v>4</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización de product backlog
</commit_message>
<xml_diff>
--- a/documentacion/Backlog.xlsx
+++ b/documentacion/Backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="19440" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>Verificar disponibilidad de laboratorio</t>
   </si>
@@ -162,9 +162,6 @@
 Registrar profesores.</t>
   </si>
   <si>
-    <t>Modelo de tabla de Computadoras</t>
-  </si>
-  <si>
     <t xml:space="preserve">Investigar el diseño de BD de una horario y su funcionamiento interno.
 </t>
   </si>
@@ -176,12 +173,37 @@
 Realizar pruebas de integración con el framework instalado.
 Diseñar un esquema de base de datos Preliminar (Bosquejo).</t>
   </si>
+  <si>
+    <t>Implementar filtros de listado en BD (laboratorio, estado)
+Diseñar la UI para mostrado de los listados</t>
+  </si>
+  <si>
+    <t>Implementar filtros de busqueda en BD (laboratorio, estado)
+Diseñar la UI para formulario y mostrado de busquedas</t>
+  </si>
+  <si>
+    <t>Diseño de UI 
+Verificar rol de acceso al metodo
+Implemetar la eliminacion en BD</t>
+  </si>
+  <si>
+    <t>Modelo de tabla de Computadoras
+Diseñar de UI Registro
+Verificar rol de acceso al metodo
+Implementar validaciones de registro de pcs
+Implementar el Registro en BD</t>
+  </si>
+  <si>
+    <t>Implemetar busqueda de laboratorios disponibles en BD
+Implementar la UI para el formulario de prestamo de laboratorios
+Realizar el registro del prestamo incluyendo el DNI del alumno en la tabla previamente creada.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +213,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -270,13 +300,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -294,6 +321,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -302,6 +332,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -318,7 +354,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -602,13 +638,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="78.42578125" bestFit="1" customWidth="1"/>
@@ -617,269 +653,291 @@
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="105">
-      <c r="A4" s="3">
+    <row r="4" spans="1:8" ht="90">
+      <c r="A4" s="2">
         <v>5</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="134.25" customHeight="1">
-      <c r="A5" s="3">
+    <row r="5" spans="1:8" ht="134.25" customHeight="1">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="90">
-      <c r="A6" s="3">
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" ht="90">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="45">
-      <c r="A7" s="3">
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" ht="45">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="45">
-      <c r="A8" s="3">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="45">
+      <c r="A8" s="2">
         <v>2</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>4</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45">
+      <c r="A9" s="2">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45">
-      <c r="A9" s="3">
-        <v>5</v>
-      </c>
-      <c r="B9" s="3">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="9" t="s">
+    <row r="10" spans="1:8" ht="60">
+      <c r="A10" s="2">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" ht="60">
+      <c r="A11" s="2">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="11"/>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30">
-      <c r="A10" s="3">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3">
-        <v>6</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" ht="60">
-      <c r="A11" s="3">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3">
-        <v>7</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="3">
-        <v>8</v>
-      </c>
-      <c r="B12" s="3">
-        <v>8</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:8">
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:8">
+      <c r="A16" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1">
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" ht="30">
+      <c r="A17" s="13">
         <v>1</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="13">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1">
+      <c r="D17" s="14"/>
+      <c r="E17" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" ht="30">
+      <c r="A18" s="13">
         <v>3</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="13">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1">
+      <c r="D18" s="14"/>
+      <c r="E18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" ht="45">
+      <c r="A19" s="13">
         <v>4</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="13">
         <v>3</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1">
+      <c r="D19" s="14"/>
+      <c r="E19" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" ht="75">
+      <c r="A20" s="13">
         <v>3</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="13">
         <v>4</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E20" t="s">
-        <v>38</v>
-      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -897,7 +955,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -909,7 +967,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>